<commit_message>
updated sonar part list with available qts
</commit_message>
<xml_diff>
--- a/sonar/amp/sonar_amp_BOM.xlsx
+++ b/sonar/amp/sonar_amp_BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
   <si>
     <t>Shematic Reference Number</t>
   </si>
@@ -274,12 +274,30 @@
   </si>
   <si>
     <t>http://www.microchip.com/mymicrochip/filehandler.aspx?ddocname=en544078</t>
+  </si>
+  <si>
+    <t>Bought</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>Used 100K instead</t>
+  </si>
+  <si>
+    <t>2 more on breakout boards</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -622,22 +640,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="1" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="25.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -659,8 +677,20 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -683,8 +713,20 @@
         <f>E2*F2</f>
         <v>0.36</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J2" s="1">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1">
+        <f>F2</f>
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <f>MAX(0,J2-K2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -707,8 +749,20 @@
         <f>E3*F3</f>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" s="1">
+        <v>10</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K22" si="0">F3</f>
+        <v>2</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" ref="L3:L22" si="1">MAX(0,J3-K3)</f>
+        <v>8</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -728,11 +782,23 @@
         <v>2</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:G11" si="0">E4*F4</f>
+        <f t="shared" ref="G4:G11" si="2">E4*F4</f>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <v>10</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -752,11 +818,23 @@
         <v>2</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J5" s="1">
+        <v>10</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -776,11 +854,23 @@
         <v>2</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J6" s="1">
+        <v>9</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -800,11 +890,23 @@
         <v>2</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J7" s="1">
+        <v>10</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -824,11 +926,23 @@
         <v>2</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J8" s="1">
+        <v>10</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -848,11 +962,23 @@
         <v>4</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1.88</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J9" s="1">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -872,11 +998,25 @@
         <v>4</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>11.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J10" s="1">
+        <v>5</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -896,11 +1036,23 @@
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2.39</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>54</v>
       </c>
@@ -920,11 +1072,23 @@
         <v>1</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" ref="G12:G22" si="1">F12*E12</f>
+        <f t="shared" ref="G12:G22" si="3">F12*E12</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>52</v>
       </c>
@@ -944,11 +1108,23 @@
         <v>2</v>
       </c>
       <c r="G13" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.84</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -968,11 +1144,22 @@
         <v>4</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.13600000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <v>6</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>59</v>
       </c>
@@ -992,11 +1179,23 @@
         <v>1</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J15" s="1">
+        <v>10</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
@@ -1016,11 +1215,23 @@
         <v>2</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.4E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" s="1">
+        <v>11</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>66</v>
       </c>
@@ -1040,11 +1251,23 @@
         <v>4</v>
       </c>
       <c r="G17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.128</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" s="1">
+        <v>16</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L17" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>71</v>
       </c>
@@ -1064,11 +1287,23 @@
         <v>1</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2000000000000001E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" s="1">
+        <v>10</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L18" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>74</v>
       </c>
@@ -1088,11 +1323,23 @@
         <v>1</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3.2000000000000001E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" s="1">
+        <v>10</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>75</v>
       </c>
@@ -1112,11 +1359,22 @@
         <v>2</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.4000000000000001E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" s="1">
+        <v>10</v>
+      </c>
+      <c r="K20" s="1">
+        <v>3</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>79</v>
       </c>
@@ -1136,11 +1394,23 @@
         <v>2</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>4.08</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" s="1">
+        <v>2</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>83</v>
       </c>
@@ -1160,34 +1430,48 @@
         <v>2</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.96</v>
+      </c>
+      <c r="J22" s="1">
+        <v>2</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="D5" r:id="rId4"/>
-    <hyperlink ref="D6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="D9" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D11" r:id="rId10"/>
-    <hyperlink ref="D12" r:id="rId11"/>
-    <hyperlink ref="D13" r:id="rId12"/>
-    <hyperlink ref="D14" r:id="rId13"/>
-    <hyperlink ref="D15" r:id="rId14"/>
-    <hyperlink ref="D16" r:id="rId15"/>
-    <hyperlink ref="D17" r:id="rId16"/>
-    <hyperlink ref="D18" r:id="rId17"/>
-    <hyperlink ref="D19" r:id="rId18"/>
-    <hyperlink ref="D20" r:id="rId19"/>
-    <hyperlink ref="D21" r:id="rId20"/>
-    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="D17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="D21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="D22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>